<commit_message>
first version of subentity migration construction
</commit_message>
<xml_diff>
--- a/ExcelSheets/Items_Markup.xlsx
+++ b/ExcelSheets/Items_Markup.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
     <t>Name</t>
   </si>
@@ -376,6 +376,54 @@
   </si>
   <si>
     <t>Checkbox</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>EntityRef</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>UpdateCriteria</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Item_Types.Type</t>
+  </si>
+  <si>
+    <t>Technological_Ages.Age</t>
+  </si>
+  <si>
+    <t>dataType</t>
+  </si>
+  <si>
+    <t>entityRef</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>updateCriteria</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>entity</t>
+  </si>
+  <si>
+    <t>checkbox</t>
   </si>
 </sst>
 </file>
@@ -759,12 +807,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51946818-A104-4834-AD3D-5CBAA30F6D00}">
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" workbookViewId="0" topLeftCell="A1">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J3" sqref="J3"/>
+      <selection pane="topRight" activeCell="B7" sqref="B7" activeCellId="0"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3" outlineLevelRow="0" defaultColWidth="8.88671875" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="15.21875" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.21875" style="1" customWidth="1"/>
@@ -776,11 +824,14 @@
     <col min="8" max="8" width="14" style="1" customWidth="1"/>
     <col min="9" max="9" width="17.44140625" style="1" customWidth="1"/>
     <col min="10" max="10" width="17.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="14" width="8.44140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="8.44140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.44140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="8.44140625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="8.44140625" style="1" customWidth="1"/>
     <col min="15" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>98</v>
       </c>
@@ -824,242 +875,216 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2">
       <c r="A2" s="1" t="s">
-        <v>99</v>
+        <v>122</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>103</v>
+        <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>107</v>
+        <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>107</v>
+        <v>2</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>107</v>
+        <v>3</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>108</v>
+        <v>11</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>112</v>
+        <v>19</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>112</v>
+        <v>15</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" ht="15">
       <c r="A3" s="1" t="s">
-        <v>100</v>
+        <v>120</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>109</v>
+        <v>127</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E4" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" t="s">
+        <v>115</v>
+      </c>
+      <c r="G5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" t="s">
+        <v>117</v>
+      </c>
+      <c r="K5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" t="s">
+        <v>93</v>
+      </c>
+      <c r="M5" t="s">
+        <v>15</v>
+      </c>
+      <c r="N5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6" s="1" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+    </row>
+    <row r="7" ht="15">
+      <c r="A7" s="1">
+        <v>-1</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="I4" s="1" t="s">
+      <c r="H7" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="K4" s="1" t="s">
+      <c r="J7" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B5" s="1">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1">
-        <v>7</v>
-      </c>
-      <c r="D5" s="2">
-        <v>7</v>
-      </c>
-      <c r="E5" s="1">
-        <v>7</v>
-      </c>
-      <c r="F5" s="1">
-        <v>7</v>
-      </c>
-      <c r="G5" s="1">
-        <v>7</v>
-      </c>
-      <c r="H5" s="1">
-        <v>7</v>
-      </c>
-      <c r="I5" s="1">
-        <v>7</v>
-      </c>
-      <c r="J5" s="1">
-        <v>7</v>
-      </c>
-      <c r="K5" s="1">
-        <v>7</v>
-      </c>
-      <c r="L5" s="1">
-        <v>7</v>
-      </c>
-      <c r="M5" s="1">
-        <v>7</v>
-      </c>
-      <c r="N5" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="1" t="s">
+    <row r="8">
+      <c r="A8" s="1">
+        <f>A7+1</f>
+        <v>0</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="E7" s="1">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1">
-        <v>2</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0</v>
-      </c>
-      <c r="H7" s="1">
-        <v>5</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
       </c>
       <c r="F8" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G8" s="1">
         <v>0</v>
       </c>
       <c r="H8" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>10</v>
@@ -1076,24 +1101,28 @@
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9">
+      <c r="A9" s="1">
+        <f>A8+1</f>
+        <v>1</v>
+      </c>
       <c r="B9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E9" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G9" s="1">
         <v>0</v>
       </c>
       <c r="H9" s="1">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>10</v>
@@ -1110,24 +1139,28 @@
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10">
+      <c r="A10" s="1">
+        <f>A9+1</f>
+        <v>2</v>
+      </c>
       <c r="B10" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2</v>
+      </c>
+      <c r="F10" s="1">
         <v>4</v>
       </c>
-      <c r="E10" s="1">
-        <v>1</v>
-      </c>
-      <c r="F10" s="1">
-        <v>5</v>
-      </c>
       <c r="G10" s="1">
         <v>0</v>
       </c>
       <c r="H10" s="1">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>10</v>
@@ -1144,24 +1177,28 @@
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11">
+      <c r="A11" s="1">
+        <f>A10+1</f>
+        <v>3</v>
+      </c>
       <c r="B11" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
       </c>
       <c r="F11" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G11" s="1">
         <v>0</v>
       </c>
       <c r="H11" s="1">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>10</v>
@@ -1178,24 +1215,28 @@
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12">
+      <c r="A12" s="1">
+        <f>A11+1</f>
+        <v>4</v>
+      </c>
       <c r="B12" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
       </c>
       <c r="F12" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G12" s="1">
         <v>0</v>
       </c>
       <c r="H12" s="1">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>10</v>
@@ -1212,27 +1253,31 @@
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13">
+      <c r="A13" s="1">
+        <f>A12+1</f>
+        <v>5</v>
+      </c>
       <c r="B13" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E13" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F13" s="1">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G13" s="1">
         <v>0</v>
       </c>
       <c r="H13" s="1">
-        <v>5</v>
+        <v>80</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>14</v>
@@ -1246,46 +1291,54 @@
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14">
+      <c r="A14" s="1">
+        <f>A13+1</f>
+        <v>6</v>
+      </c>
       <c r="B14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="1">
+        <v>5</v>
+      </c>
+      <c r="F14" s="1">
+        <v>4</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>5</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
+        <f>A14+1</f>
+        <v>7</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="E14" s="1">
-        <v>0</v>
-      </c>
-      <c r="F14" s="1">
-        <v>0</v>
-      </c>
-      <c r="G14" s="1">
-        <v>2</v>
-      </c>
-      <c r="H14" s="1">
-        <v>16</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B15" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="E15" s="1">
         <v>0</v>
@@ -1297,46 +1350,50 @@
         <v>2</v>
       </c>
       <c r="H15" s="1">
+        <v>16</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1">
+        <f>A15+1</f>
+        <v>8</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <v>2</v>
+      </c>
+      <c r="H16" s="1">
         <v>10</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="N15" s="3"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="1">
-        <v>0</v>
-      </c>
-      <c r="F16" s="1">
-        <v>0</v>
-      </c>
-      <c r="G16" s="1">
-        <v>3</v>
-      </c>
-      <c r="H16" s="4">
-        <v>20</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J16" s="4" t="s">
+      <c r="J16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="K16" s="3" t="s">
@@ -1348,48 +1405,58 @@
       </c>
       <c r="N16" s="3"/>
     </row>
-    <row r="17" spans="2:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17">
+      <c r="A17" s="1">
+        <f>A16+1</f>
+        <v>9</v>
+      </c>
       <c r="B17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>3</v>
+      </c>
+      <c r="H17" s="4">
+        <v>20</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N17" s="3"/>
+    </row>
+    <row r="18" ht="42">
+      <c r="A18" s="1">
+        <f>A17+1</f>
+        <v>10</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="1">
-        <v>0</v>
-      </c>
-      <c r="F17" s="1">
-        <v>0</v>
-      </c>
-      <c r="G17" s="1">
-        <v>0</v>
-      </c>
-      <c r="H17" s="1">
-        <v>30</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B18" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="E18" s="1">
         <v>0</v>
       </c>
@@ -1397,13 +1464,13 @@
         <v>0</v>
       </c>
       <c r="G18" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H18" s="1">
         <v>30</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>14</v>
@@ -1412,17 +1479,19 @@
         <v>20</v>
       </c>
       <c r="L18" s="3"/>
-      <c r="M18" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="M18" s="3"/>
       <c r="N18" s="3"/>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="19">
+      <c r="A19" s="1">
+        <f>A18+1</f>
+        <v>11</v>
+      </c>
       <c r="B19" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E19" s="1">
         <v>0</v>
@@ -1431,10 +1500,10 @@
         <v>0</v>
       </c>
       <c r="G19" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H19" s="1">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>15</v>
@@ -1451,12 +1520,16 @@
       </c>
       <c r="N19" s="3"/>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="20">
+      <c r="A20" s="1">
+        <f>A19+1</f>
+        <v>12</v>
+      </c>
       <c r="B20" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E20" s="1">
         <v>0</v>
@@ -1465,10 +1538,10 @@
         <v>0</v>
       </c>
       <c r="G20" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H20" s="1">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>15</v>
@@ -1485,58 +1558,66 @@
       </c>
       <c r="N20" s="3"/>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="21">
+      <c r="A21" s="1">
+        <f>A20+1</f>
+        <v>13</v>
+      </c>
       <c r="B21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1">
+        <v>5</v>
+      </c>
+      <c r="H21" s="1">
+        <v>80</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N21" s="3"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="1">
+        <f>A21+1</f>
+        <v>14</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="E21" s="1">
-        <v>1</v>
-      </c>
-      <c r="F21" s="5">
-        <v>9</v>
-      </c>
-      <c r="G21" s="5">
-        <v>0</v>
-      </c>
-      <c r="H21" s="5">
-        <v>80</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B22" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="E22" s="1">
         <v>1</v>
       </c>
       <c r="F22" s="5">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G22" s="5">
         <v>0</v>
       </c>
       <c r="H22" s="5">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>10</v>
@@ -1553,24 +1634,28 @@
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="23">
+      <c r="A23" s="1">
+        <f>A22+1</f>
+        <v>15</v>
+      </c>
       <c r="B23" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E23" s="1">
         <v>1</v>
       </c>
       <c r="F23" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G23" s="5">
         <v>0</v>
       </c>
       <c r="H23" s="5">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>10</v>
@@ -1587,30 +1672,31 @@
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="24">
+      <c r="A24" s="1">
+        <f>A23+1</f>
+        <v>16</v>
+      </c>
       <c r="B24" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E24" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F24" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G24" s="5">
         <v>0</v>
       </c>
       <c r="H24" s="5">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>14</v>
@@ -1624,27 +1710,31 @@
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="25">
+      <c r="A25" s="1">
+        <f>A24+1</f>
+        <v>17</v>
+      </c>
       <c r="B25" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>60</v>
       </c>
       <c r="E25" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F25" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G25" s="5">
         <v>0</v>
       </c>
       <c r="H25" s="5">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>13</v>
@@ -1661,27 +1751,31 @@
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="26">
+      <c r="A26" s="1">
+        <f>A25+1</f>
+        <v>18</v>
+      </c>
       <c r="B26" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E26" s="1">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F26" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G26" s="5">
         <v>0</v>
       </c>
       <c r="H26" s="5">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>13</v>
@@ -1698,27 +1792,31 @@
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="27">
+      <c r="A27" s="1">
+        <f>A26+1</f>
+        <v>19</v>
+      </c>
       <c r="B27" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E27" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F27" s="5">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G27" s="5">
         <v>0</v>
       </c>
       <c r="H27" s="5">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>13</v>
@@ -1735,18 +1833,22 @@
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="28">
+      <c r="A28" s="1">
+        <f>A27+1</f>
+        <v>20</v>
+      </c>
       <c r="B28" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E28" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F28" s="5">
         <v>9</v>
@@ -1755,7 +1857,7 @@
         <v>0</v>
       </c>
       <c r="H28" s="5">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>13</v>
@@ -1772,27 +1874,31 @@
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="29">
+      <c r="A29" s="1">
+        <f>A28+1</f>
+        <v>21</v>
+      </c>
       <c r="B29" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E29" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F29" s="5">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G29" s="5">
         <v>0</v>
       </c>
       <c r="H29" s="5">
-        <v>180</v>
+        <v>140</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>13</v>
@@ -1809,52 +1915,69 @@
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="30">
+      <c r="A30" s="1">
+        <f>A29+1</f>
+        <v>22</v>
+      </c>
       <c r="B30" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E30" s="1">
+        <v>10</v>
+      </c>
+      <c r="F30" s="5">
+        <v>12</v>
+      </c>
+      <c r="G30" s="5">
+        <v>0</v>
+      </c>
+      <c r="H30" s="5">
+        <v>180</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="1">
+        <f>A30+1</f>
+        <v>23</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F30" s="5">
-        <v>0</v>
-      </c>
-      <c r="G30" s="5">
+      <c r="F31" s="5">
+        <v>0</v>
+      </c>
+      <c r="G31" s="5">
         <v>2</v>
       </c>
-      <c r="H30" s="5">
+      <c r="H31" s="5">
         <v>30</v>
       </c>
-      <c r="I30" s="1" t="s">
+      <c r="I31" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K30" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="2:14" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B31" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H31" s="5">
-        <v>60</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>14</v>
@@ -1864,17 +1987,23 @@
       </c>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
-    </row>
-    <row r="32" spans="2:14" ht="72" x14ac:dyDescent="0.3">
+      <c r="N31" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" ht="57">
+      <c r="A32" s="1">
+        <f>A31+1</f>
+        <v>24</v>
+      </c>
       <c r="B32" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H32" s="5">
         <v>60</v>
@@ -1892,21 +2021,22 @@
       <c r="M32" s="3"/>
       <c r="N32" s="3"/>
     </row>
-    <row r="33" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" ht="72">
+      <c r="A33" s="1">
+        <f>A32+1</f>
+        <v>25</v>
+      </c>
       <c r="B33" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E33" s="1">
-        <v>5</v>
+        <v>91</v>
       </c>
       <c r="H33" s="5">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>23</v>
@@ -1921,24 +2051,28 @@
       <c r="M33" s="3"/>
       <c r="N33" s="3"/>
     </row>
-    <row r="34" spans="2:14" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="34" ht="28">
+      <c r="A34" s="1">
+        <f>A33+1</f>
+        <v>26</v>
+      </c>
       <c r="B34" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="E34" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H34" s="5">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>74</v>
+        <v>23</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>14</v>
@@ -1950,18 +2084,25 @@
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>
     </row>
-    <row r="35" spans="2:14" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="35" ht="57">
+      <c r="A35" s="1">
+        <f>A34+1</f>
+        <v>27</v>
+      </c>
       <c r="B35" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
+      </c>
+      <c r="E35" s="1">
+        <v>1</v>
       </c>
       <c r="H35" s="5">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>74</v>
@@ -1976,18 +2117,22 @@
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
     </row>
-    <row r="36" spans="2:14" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="36" ht="86">
+      <c r="A36" s="1">
+        <f>A35+1</f>
+        <v>28</v>
+      </c>
       <c r="B36" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H36" s="5">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>74</v>
@@ -2002,18 +2147,22 @@
       <c r="M36" s="3"/>
       <c r="N36" s="3"/>
     </row>
-    <row r="37" spans="2:14" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="37" ht="57">
+      <c r="A37" s="1">
+        <f>A36+1</f>
+        <v>29</v>
+      </c>
       <c r="B37" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H37" s="5">
-        <v>80</v>
+        <v>35</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>74</v>
@@ -2028,18 +2177,22 @@
       <c r="M37" s="3"/>
       <c r="N37" s="3"/>
     </row>
-    <row r="38" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" ht="100">
+      <c r="A38" s="1">
+        <f>A37+1</f>
+        <v>30</v>
+      </c>
       <c r="B38" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C38" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H38" s="5">
         <v>80</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="H38" s="5">
-        <v>25</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>74</v>
@@ -2054,18 +2207,22 @@
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
     </row>
-    <row r="39" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" ht="28">
+      <c r="A39" s="1">
+        <f>A38+1</f>
+        <v>31</v>
+      </c>
       <c r="B39" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H39" s="5">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>74</v>
@@ -2079,6 +2236,36 @@
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
+    </row>
+    <row r="40" ht="28">
+      <c r="A40" s="1">
+        <f>A39+1</f>
+        <v>32</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H40" s="5">
+        <v>50</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
take finished logic and move it to a library file
</commit_message>
<xml_diff>
--- a/ExcelSheets/Items_Markup.xlsx
+++ b/ExcelSheets/Items_Markup.xlsx
@@ -424,6 +424,9 @@
   </si>
   <si>
     <t>checkbox</t>
+  </si>
+  <si>
+    <t>active</t>
   </si>
 </sst>
 </file>
@@ -809,7 +812,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" workbookViewId="0" topLeftCell="A1">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B7" sqref="B7" activeCellId="0"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1" activeCellId="0"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3" outlineLevelRow="0" defaultColWidth="8.88671875" outlineLevelCol="0"/>
@@ -833,7 +836,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>98</v>
+        <v>129</v>
       </c>
       <c r="B1" s="1" t="b">
         <v>1</v>

</xml_diff>